<commit_message>
Registe a customer Test case completion.
</commit_message>
<xml_diff>
--- a/HybridFramework/src/test/resources/CustomerDetails.xlsx
+++ b/HybridFramework/src/test/resources/CustomerDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation-Framework\HybridFramework\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation Framework\Hybrid_Framework\HybridFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26AA510-705F-43F3-BAD2-8BD207488E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22ECBA2E-2784-41E8-8D5E-7139FB72C662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,10 @@
     <t>Uttar Pradesh</t>
   </si>
   <si>
-    <t>Aj2002</t>
-  </si>
-  <si>
     <t>Arshad$2025</t>
+  </si>
+  <si>
+    <t>Ars2001</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,13 +468,13 @@
         <v>1254567</v>
       </c>
       <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>